<commit_message>
Added script for bme280 calibration
</commit_message>
<xml_diff>
--- a/data/20200214-140824-thin_orange_foam_side_vaseline_only.xlsx
+++ b/data/20200214-140824-thin_orange_foam_side_vaseline_only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6e372e5b8c96f59/stom/systems/vacuum_meter/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mh/OneDrive/stom/systems/vacuum_meter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:4000b_{95ED2109-C7CF-7D48-8737-01665183082D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200214-140824-thin_orange_foa" sheetId="1" r:id="rId1"/>
@@ -1931,7 +1931,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -6585,6 +6585,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="155715599"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -7268,15 +7269,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C630" totalsRowShown="0">
-  <autoFilter ref="A1:C630"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C630" totalsRowShown="0">
+  <autoFilter ref="A1:C630" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C630">
     <sortCondition ref="A1:A630"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="timestamp"/>
-    <tableColumn id="2" name="load"/>
-    <tableColumn id="3" name="pressure"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="timestamp"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="load"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="pressure"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7578,11 +7579,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C630"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>